<commit_message>
Dev: Add DateAdapter and unit test.
</commit_message>
<xml_diff>
--- a/src/test/resources/Student.xlsx
+++ b/src/test/resources/Student.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,6 +82,10 @@
   </si>
   <si>
     <t>Swimming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Birth</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -95,6 +99,7 @@
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -124,8 +129,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -462,15 +468,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,8 +489,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -497,8 +506,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="1">
+        <v>43467</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -511,8 +523,11 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
+      <c r="E3" s="1">
+        <v>43468</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -525,8 +540,11 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
+      <c r="E4" s="1">
+        <v>43469</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -539,8 +557,11 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
+      <c r="E5" s="1">
+        <v>43470</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -552,6 +573,9 @@
       </c>
       <c r="D6" t="s">
         <v>12</v>
+      </c>
+      <c r="E6" s="1">
+        <v>43471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>